<commit_message>
add new geocoded family medicine providers to the dataset.
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -12659,7 +12659,7 @@
       </c>
       <c r="G255" t="inlineStr">
         <is>
-          <t>Calea DudeSti 104-122, Sector 3, Bucuresti</t>
+          <t>, Bucuresti</t>
         </is>
       </c>
       <c r="H255" t="inlineStr">
@@ -14291,7 +14291,7 @@
       </c>
       <c r="G289" t="inlineStr">
         <is>
-          <t>Bulevardul ul Agronom Ion Ionescu de la Brad, 1A, Sector 1, Bucuresti</t>
+          <t>Bulevardul Agronom Ion Ionescu de la Brad, 1A, Sector 1, Bucuresti</t>
         </is>
       </c>
       <c r="H289" t="inlineStr">
@@ -14339,7 +14339,7 @@
       </c>
       <c r="G290" t="inlineStr">
         <is>
-          <t>Bulevardul ul Agronom Ion Ionescu de la Brad, 1A, Sector 1, Bucuresti</t>
+          <t>Bulevardul Agronom Ion Ionescu de la Brad, 1A, Sector 1, Bucuresti</t>
         </is>
       </c>
       <c r="H290" t="inlineStr">
@@ -16115,7 +16115,7 @@
       </c>
       <c r="G327" t="inlineStr">
         <is>
-          <t>Strada Erou Ion Calea in, 37, Sector 2, Bucuresti</t>
+          <t>Strada Erou Ion Calin, 37, Sector 2, Bucuresti</t>
         </is>
       </c>
       <c r="H327" t="inlineStr">
@@ -16163,7 +16163,7 @@
       </c>
       <c r="G328" t="inlineStr">
         <is>
-          <t>Strada Erou Ion Calea in, 37, Sector 2, Bucuresti</t>
+          <t>Strada Erou Ion Calin, 37, Sector 2, Bucuresti</t>
         </is>
       </c>
       <c r="H328" t="inlineStr">
@@ -16211,7 +16211,7 @@
       </c>
       <c r="G329" t="inlineStr">
         <is>
-          <t>Strada Erou Ion Calea in, 37, Sector 2, Bucuresti</t>
+          <t>Strada Erou Ion Calin, 37, Sector 2, Bucuresti</t>
         </is>
       </c>
       <c r="H329" t="inlineStr">
@@ -17219,7 +17219,7 @@
       </c>
       <c r="G350" t="inlineStr">
         <is>
-          <t>Strada Dr.Calea istrat Grozovici 6, Sector 2, Bucuresti</t>
+          <t>Strada Dr.Calistrat Grozovici 6, Sector 2, Bucuresti</t>
         </is>
       </c>
       <c r="H350" t="inlineStr">
@@ -17267,7 +17267,7 @@
       </c>
       <c r="G351" t="inlineStr">
         <is>
-          <t>Strada Dr.Calea istrat Grozovici 6, Sector 2, Bucuresti</t>
+          <t>Strada Dr.Calistrat Grozovici 6, Sector 2, Bucuresti</t>
         </is>
       </c>
       <c r="H351" t="inlineStr">
@@ -17315,7 +17315,7 @@
       </c>
       <c r="G352" t="inlineStr">
         <is>
-          <t>Strada Dr.Calea istrat Grozovici 6, Sector 2, Bucuresti</t>
+          <t>Strada Dr.Calistrat Grozovici 6, Sector 2, Bucuresti</t>
         </is>
       </c>
       <c r="H352" t="inlineStr">
@@ -17363,7 +17363,7 @@
       </c>
       <c r="G353" t="inlineStr">
         <is>
-          <t>Strada Dr.Calea istrat Grozovici 6, Sector 2, Bucuresti</t>
+          <t>Strada Dr.Calistrat Grozovici 6, Sector 2, Bucuresti</t>
         </is>
       </c>
       <c r="H353" t="inlineStr">
@@ -17411,7 +17411,7 @@
       </c>
       <c r="G354" t="inlineStr">
         <is>
-          <t>Strada Dr. Calea istrat Grozovici, 6, Sector 2, Bucuresti</t>
+          <t>Strada Dr. Calistrat Grozovici, 6, Sector 2, Bucuresti</t>
         </is>
       </c>
       <c r="H354" t="inlineStr">
@@ -20051,7 +20051,7 @@
       </c>
       <c r="G409" t="inlineStr">
         <is>
-          <t>Aleea Calea istrat Hogas, 45B, Sector 3, Bucuresti</t>
+          <t>Aleea Calistrat Hogas, 45B, Sector 3, Bucuresti</t>
         </is>
       </c>
       <c r="H409" t="inlineStr">
@@ -20771,7 +20771,7 @@
       </c>
       <c r="G424" t="inlineStr">
         <is>
-          <t>Strada Jean Luis Calea deron, 45, Sector 2, Bucuresti</t>
+          <t>Strada Jean Luis Calderon, 45, Sector 2, Bucuresti</t>
         </is>
       </c>
       <c r="H424" t="inlineStr">
@@ -21299,7 +21299,7 @@
       </c>
       <c r="G435" t="inlineStr">
         <is>
-          <t>Aleea Calea istrat Hogas, 45B, Sector 3, Bucuresti</t>
+          <t>Aleea Calistrat Hogas, 45B, Sector 3, Bucuresti</t>
         </is>
       </c>
       <c r="H435" t="inlineStr">
@@ -21923,7 +21923,7 @@
       </c>
       <c r="G448" t="inlineStr">
         <is>
-          <t>Calea 13 Septembrie 197, Sector 5, Bucuresti</t>
+          <t>, Bucuresti</t>
         </is>
       </c>
       <c r="H448" t="inlineStr">
@@ -30707,7 +30707,7 @@
       </c>
       <c r="G631" t="inlineStr">
         <is>
-          <t>Strada Calea istrat Grozovici, 6, Sector 2, Bucuresti</t>
+          <t>Strada Calistrat Grozovici, 6, Sector 2, Bucuresti</t>
         </is>
       </c>
       <c r="H631" t="inlineStr">
@@ -30851,7 +30851,7 @@
       </c>
       <c r="G634" t="inlineStr">
         <is>
-          <t>Strada Dr. Calea istrat Grozovici, 6, Sector 2, Bucuresti</t>
+          <t>Strada Dr. Calistrat Grozovici, 6, Sector 2, Bucuresti</t>
         </is>
       </c>
       <c r="H634" t="inlineStr">
@@ -33395,7 +33395,7 @@
       </c>
       <c r="G687" t="inlineStr">
         <is>
-          <t>Calea Calea arasilor, 177, Sector 3, Bucuresti</t>
+          <t>Calea Calarasilor, 177, Sector 3, Bucuresti</t>
         </is>
       </c>
       <c r="H687" t="inlineStr">
@@ -33443,7 +33443,7 @@
       </c>
       <c r="G688" t="inlineStr">
         <is>
-          <t>Calea Calea arasilor, 177, Sector 3, Bucuresti</t>
+          <t>Calea Calarasilor, 177, Sector 3, Bucuresti</t>
         </is>
       </c>
       <c r="H688" t="inlineStr">
@@ -38141,7 +38141,7 @@
       </c>
       <c r="G786" t="inlineStr">
         <is>
-          <t>Strada Dr. Calea istrat Grozovici, 6, Sector 2, Bucuresti</t>
+          <t>Strada Dr. Calistrat Grozovici, 6, Sector 2, Bucuresti</t>
         </is>
       </c>
       <c r="H786" t="inlineStr">
@@ -39915,7 +39915,7 @@
       </c>
       <c r="G823" t="inlineStr">
         <is>
-          <t>Strada Dr. Calea istrat Grozovici, 6, Sector 2, Bucuresti</t>
+          <t>Strada Dr. Calistrat Grozovici, 6, Sector 2, Bucuresti</t>
         </is>
       </c>
       <c r="H823" t="inlineStr">
@@ -41163,7 +41163,7 @@
       </c>
       <c r="G849" t="inlineStr">
         <is>
-          <t>Calea Calea arasilor, 175, Sector 3, Bucuresti</t>
+          <t>Calea Calarasilor, 175, Sector 3, Bucuresti</t>
         </is>
       </c>
       <c r="H849" t="inlineStr">
@@ -41211,7 +41211,7 @@
       </c>
       <c r="G850" t="inlineStr">
         <is>
-          <t>Calea Calea arasilor, 175, Sector 3, Bucuresti</t>
+          <t>Calea Calarasilor, 175, Sector 3, Bucuresti</t>
         </is>
       </c>
       <c r="H850" t="inlineStr">
@@ -41883,7 +41883,7 @@
       </c>
       <c r="G864" t="inlineStr">
         <is>
-          <t>Strada Ottoi Calea in, 20-22, Sector 2, Bucuresti</t>
+          <t>Strada Ottoi Calin, 20-22, Sector 2, Bucuresti</t>
         </is>
       </c>
       <c r="H864" t="inlineStr">
@@ -48747,7 +48747,7 @@
       </c>
       <c r="G1007" t="inlineStr">
         <is>
-          <t>Calea Calea arasilor, 175, Sector 3, Bucuresti</t>
+          <t>Calea Calarasilor, 175, Sector 3, Bucuresti</t>
         </is>
       </c>
       <c r="H1007" t="inlineStr">

</xml_diff>

<commit_message>
introduce a `--reset` option to `geocode_interactive_fix.py` for clearing coordinates, manual addresses, and cache entries for specified addresses.
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -20056,14 +20056,14 @@
       </c>
       <c r="H409" t="inlineStr">
         <is>
-          <t>calistrat hogas, 45</t>
+          <t>aleea calistrat hogas, 45b, sector 3, bucuresti</t>
         </is>
       </c>
       <c r="I409" t="n">
-        <v>46.0946119</v>
+        <v>44.421862</v>
       </c>
       <c r="J409" t="n">
-        <v>23.5562449</v>
+        <v>26.1737386</v>
       </c>
     </row>
     <row r="410">
@@ -21304,14 +21304,14 @@
       </c>
       <c r="H435" t="inlineStr">
         <is>
-          <t>calistrat hogas, 45</t>
+          <t>Aleea Calistrat Hogas, 45B, Sector 3, Bucuresti</t>
         </is>
       </c>
       <c r="I435" t="n">
-        <v>46.0946119</v>
+        <v>44.421862</v>
       </c>
       <c r="J435" t="n">
-        <v>23.5562449</v>
+        <v>26.1737386</v>
       </c>
     </row>
     <row r="436">
@@ -22936,14 +22936,14 @@
       </c>
       <c r="H469" t="inlineStr">
         <is>
-          <t>calea victoriei, 14</t>
+          <t>calea victoriei, 14, sector 3, bucuresti</t>
         </is>
       </c>
       <c r="I469" t="n">
-        <v>46.1850942</v>
+        <v>44.432793</v>
       </c>
       <c r="J469" t="n">
-        <v>21.3100461</v>
+        <v>26.0976684</v>
       </c>
     </row>
     <row r="470">

</xml_diff>